<commit_message>
added deviation and AIC information for models including location variable
</commit_message>
<xml_diff>
--- a/Best_Models.xlsx
+++ b/Best_Models.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="146">
   <si>
     <t>No. Model</t>
   </si>
@@ -511,9 +511,6 @@
     <t>Model31Sector</t>
   </si>
   <si>
-    <t>0.001693 **</t>
-  </si>
-  <si>
     <t>Model31UAC</t>
   </si>
   <si>
@@ -526,9 +523,6 @@
     <t>Model36Sector</t>
   </si>
   <si>
-    <t>0.002135 **</t>
-  </si>
-  <si>
     <t>Model36UAC</t>
   </si>
   <si>
@@ -544,9 +538,6 @@
     <t>Model38Sector</t>
   </si>
   <si>
-    <t>0.0008654 ***</t>
-  </si>
-  <si>
     <t>Model38UAC</t>
   </si>
   <si>
@@ -559,9 +550,6 @@
     <t>Model43Sector</t>
   </si>
   <si>
-    <t>0.001284 **</t>
-  </si>
-  <si>
     <t>Model43UAC</t>
   </si>
   <si>
@@ -584,15 +572,37 @@
   </si>
   <si>
     <t>Model27UAC_Sector</t>
+  </si>
+  <si>
+    <t>0,0007979***</t>
+  </si>
+  <si>
+    <t>0,01216*</t>
+  </si>
+  <si>
+    <t>0.002053 **</t>
+  </si>
+  <si>
+    <t>0,003663**</t>
+  </si>
+  <si>
+    <t>0,04252*</t>
+  </si>
+  <si>
+    <t>0,0009484***</t>
+  </si>
+  <si>
+    <t>0,003394**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -754,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -840,157 +850,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1007,7 +870,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,6 +893,154 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,7 +1323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -1373,27 +1384,27 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="47">
+      <c r="C2" s="79"/>
+      <c r="D2" s="63">
         <f>46-6</f>
         <v>40</v>
       </c>
-      <c r="E2" s="61">
+      <c r="E2" s="66">
         <v>0.35859999999999997</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="90">
         <v>0.48899999999999999</v>
       </c>
-      <c r="H2" s="47">
+      <c r="H2" s="63">
         <v>6.452</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -1408,100 +1419,100 @@
       <c r="L2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="54"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="47"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="62"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="41" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="48"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="64"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="62"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="53"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="48"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="64"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="49"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="65"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63">
         <v>40</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="66">
         <v>0.35299999999999998</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="47">
+      <c r="G6" s="63">
         <v>0.49299999999999999</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="63">
         <v>5.2560000000000002</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -1516,122 +1527,122 @@
       <c r="L6" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="47"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="63"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="62"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="67"/>
       <c r="F7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="41" t="s">
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="K7" s="70" t="s">
+      <c r="K7" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="70" t="s">
+      <c r="L7" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="48"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="64"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="62"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="67"/>
       <c r="F8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="48"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="64"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="62"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="48"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="64"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="63"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="46"/>
-      <c r="N10" s="46"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="49"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="65"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="63">
         <v>40</v>
       </c>
-      <c r="E11" s="61">
+      <c r="E11" s="66">
         <v>0.55869999999999997</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="63">
         <v>7.1100000000000004E-4</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="63">
         <v>13.34</v>
       </c>
       <c r="I11" s="14" t="s">
@@ -1652,26 +1663,26 @@
       <c r="P11" s="11"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="62"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="41" t="s">
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="78" t="s">
+      <c r="K12" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="78" t="s">
+      <c r="L12" s="73" t="s">
         <v>68</v>
       </c>
       <c r="M12" s="10"/>
@@ -1680,68 +1691,68 @@
       <c r="P12" s="11"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="62"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="67"/>
       <c r="F13" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
       <c r="M13" s="10"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="11"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="63"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="80"/>
-      <c r="L14" s="80"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
       <c r="M14" s="10"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="11"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="63">
         <v>40</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="63">
         <v>0.45069999999999999</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="90">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H15" s="47">
+      <c r="H15" s="63">
         <v>9</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -1756,102 +1767,102 @@
       <c r="L15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="M15" s="54"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44"/>
-      <c r="P15" s="47"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="63"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
       <c r="F16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="53"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="41" t="s">
+      <c r="G16" s="90"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="K16" s="70" t="s">
+      <c r="K16" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="L16" s="41" t="s">
+      <c r="L16" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="M16" s="54"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="48"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="64"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
       <c r="F17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="53"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="48"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="64"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
+      <c r="A18" s="65"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
       <c r="F18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="53"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="46"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="49"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="65"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="63">
         <v>40</v>
       </c>
-      <c r="E19" s="47">
+      <c r="E19" s="63">
         <v>0.46750000000000003</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="63">
         <v>0.40600000000000003</v>
       </c>
-      <c r="H19" s="47">
+      <c r="H19" s="63">
         <v>9.5609999999999999</v>
       </c>
       <c r="I19" s="6" t="s">
@@ -1872,26 +1883,26 @@
       <c r="P19" s="11"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="41" t="s">
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="41" t="s">
+      <c r="J20" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="70" t="s">
+      <c r="K20" s="76" t="s">
         <v>92</v>
       </c>
-      <c r="L20" s="41" t="s">
+      <c r="L20" s="69" t="s">
         <v>84</v>
       </c>
       <c r="M20" s="9"/>
@@ -1900,78 +1911,78 @@
       <c r="P20" s="11"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
       <c r="F21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="64">
         <v>0.52600000000000002</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="64">
         <v>5.141</v>
       </c>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="47"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="77"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="72"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="63"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="A22" s="65"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
       <c r="F22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="43" t="s">
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="72"/>
-      <c r="L22" s="43" t="s">
+      <c r="K22" s="78"/>
+      <c r="L22" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="M22" s="54"/>
-      <c r="N22" s="46"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="49"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="65"/>
     </row>
     <row r="23" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
+      <c r="A23" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="67">
+      <c r="D23" s="83">
         <v>40</v>
       </c>
-      <c r="E23" s="67">
+      <c r="E23" s="83">
         <v>0.35720000000000002</v>
       </c>
       <c r="F23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="77">
+      <c r="G23" s="89">
         <v>0.49</v>
       </c>
-      <c r="H23" s="67">
+      <c r="H23" s="83">
         <v>8.2240000000000002</v>
       </c>
       <c r="I23" s="7" t="s">
@@ -1986,82 +1997,82 @@
       <c r="L23" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="M23" s="73"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="67"/>
+      <c r="M23" s="82"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+      <c r="P23" s="83"/>
     </row>
     <row r="24" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="68"/>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
+      <c r="A24" s="84"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="84"/>
+      <c r="E24" s="84"/>
       <c r="F24" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="77"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="41" t="s">
+      <c r="G24" s="89"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="41" t="s">
+      <c r="J24" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="L24" s="70" t="s">
+      <c r="L24" s="76" t="s">
         <v>94</v>
       </c>
-      <c r="M24" s="73"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="68"/>
+      <c r="M24" s="82"/>
+      <c r="N24" s="92"/>
+      <c r="O24" s="92"/>
+      <c r="P24" s="84"/>
     </row>
     <row r="25" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
       <c r="F25" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="77"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="66"/>
-      <c r="O25" s="66"/>
-      <c r="P25" s="69"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="93"/>
+      <c r="O25" s="93"/>
+      <c r="P25" s="85"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="50" t="s">
+      <c r="C26" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="67">
+      <c r="D26" s="83">
         <v>40</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="63">
         <v>0.45069999999999999</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="53">
+      <c r="G26" s="90">
         <v>0.41899999999999998</v>
       </c>
-      <c r="H26" s="47">
+      <c r="H26" s="63">
         <v>11.67</v>
       </c>
       <c r="I26" s="6" t="s">
@@ -2076,140 +2087,61 @@
       <c r="L26" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="M26" s="54"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
-      <c r="P26" s="47"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="63"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="48"/>
+      <c r="A27" s="64"/>
+      <c r="B27" s="80"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="53"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="41" t="s">
+      <c r="G27" s="90"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="J27" s="41" t="s">
+      <c r="J27" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="K27" s="41" t="s">
+      <c r="K27" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="41" t="s">
+      <c r="L27" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="M27" s="54"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="48"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="64"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="49"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="49"/>
+      <c r="A28" s="65"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="65"/>
       <c r="F28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="54"/>
-      <c r="N28" s="46"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="49"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="O6:O10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="J12:J14"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="K20:K22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="M26:M28"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="H19:H22"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="N26:N28"/>
-    <mergeCell ref="O26:O28"/>
-    <mergeCell ref="P26:P28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="N23:N25"/>
-    <mergeCell ref="O23:O25"/>
-    <mergeCell ref="P23:P25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="M2:M5"/>
-    <mergeCell ref="N2:N5"/>
-    <mergeCell ref="O2:O5"/>
-    <mergeCell ref="P2:P5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="O15:O18"/>
     <mergeCell ref="P15:P18"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="B15:B18"/>
@@ -2232,6 +2164,85 @@
     <mergeCell ref="L7:L10"/>
     <mergeCell ref="M6:M10"/>
     <mergeCell ref="N6:N10"/>
+    <mergeCell ref="M2:M5"/>
+    <mergeCell ref="N2:N5"/>
+    <mergeCell ref="O2:O5"/>
+    <mergeCell ref="P2:P5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="N23:N25"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="P23:P25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="P26:P28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="K20:K22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="M26:M28"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="H19:H22"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="O6:O10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="O15:O18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2242,7 +2253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -2253,45 +2264,46 @@
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" style="108" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="59" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="100" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="89" t="s">
+      <c r="D1" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="100" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="100" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="89" t="s">
+      <c r="G1" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
     </row>
     <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="103" t="s">
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="54" t="s">
         <v>108</v>
       </c>
       <c r="H2" s="21" t="s">
@@ -2305,81 +2317,81 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87">
+      <c r="A3" s="101">
         <v>26</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="102" t="s">
         <v>42</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="92">
+      <c r="D3" s="43">
         <v>91.572999999999993</v>
       </c>
-      <c r="E3" s="91">
+      <c r="E3" s="42">
         <v>29.745999999999999</v>
       </c>
-      <c r="F3" s="91">
+      <c r="F3" s="41">
         <v>17.120999999999999</v>
       </c>
-      <c r="G3" s="104"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="25"/>
       <c r="I3" s="26"/>
       <c r="J3" s="27">
-        <f t="shared" ref="J3:J18" si="0">+((E3-F3)/E3)*100</f>
+        <f>+((E3-F3)/E3)*100</f>
         <v>42.442681368923559</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="88"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="102"/>
       <c r="C4" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="97">
+      <c r="D4" s="48">
         <v>60.006</v>
       </c>
-      <c r="E4" s="98">
+      <c r="E4" s="49">
         <v>29.745999999999999</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="50">
         <v>3.8618999999999999</v>
       </c>
-      <c r="G4" s="104">
+      <c r="G4" s="56">
         <f>+F3-F4</f>
         <v>13.259099999999998</v>
       </c>
-      <c r="H4" s="100">
+      <c r="H4" s="51">
         <v>5.1501000000000001</v>
       </c>
-      <c r="I4" s="100" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" s="101">
-        <f t="shared" si="0"/>
+      <c r="I4" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="52">
+        <f t="shared" ref="J3:J18" si="0">+((E4-F4)/E4)*100</f>
         <v>87.017077926443903</v>
       </c>
-      <c r="K4" s="102">
+      <c r="K4" s="53">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
-      <c r="B5" s="88"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="23" t="s">
         <v>113</v>
       </c>
       <c r="D5" s="24">
         <v>85.554000000000002</v>
       </c>
-      <c r="E5" s="91">
+      <c r="E5" s="42">
         <v>29.745999999999999</v>
       </c>
-      <c r="F5" s="90">
+      <c r="F5" s="41">
         <v>12.06</v>
       </c>
-      <c r="G5" s="105">
+      <c r="G5" s="56">
         <f>+F3-F5</f>
         <v>5.0609999999999982</v>
       </c>
@@ -2387,32 +2399,32 @@
         <v>3.2528999999999999</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J5" s="27">
         <f t="shared" si="0"/>
         <v>59.456733678477782</v>
       </c>
-      <c r="K5" s="95">
+      <c r="K5" s="46">
         <v>0.95</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="87"/>
-      <c r="B6" s="88"/>
+      <c r="A6" s="101"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="93">
+      <c r="D6" s="44">
         <v>60.006</v>
       </c>
-      <c r="E6" s="91">
+      <c r="E6" s="42">
         <v>29.745999999999999</v>
       </c>
-      <c r="F6" s="94">
+      <c r="F6" s="45">
         <v>3.8618999999999999</v>
       </c>
-      <c r="G6" s="105">
+      <c r="G6" s="56">
         <f>+F3-F6</f>
         <v>13.259099999999998</v>
       </c>
@@ -2420,484 +2432,607 @@
         <v>5.1501000000000001</v>
       </c>
       <c r="I6" s="34" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J6" s="35">
         <f t="shared" si="0"/>
         <v>87.017077926443903</v>
       </c>
-      <c r="K6" s="96">
+      <c r="K6" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81">
+      <c r="A7" s="103">
         <v>27</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="106" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D7" s="34">
         <v>92.760999999999996</v>
       </c>
-      <c r="E7" s="91">
+      <c r="E7" s="42">
         <v>29.745999999999999</v>
       </c>
-      <c r="F7" s="94">
+      <c r="F7" s="45">
         <v>16.777000000000001</v>
       </c>
-      <c r="G7" s="105"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="34"/>
       <c r="I7" s="34"/>
       <c r="J7" s="35">
+        <f>+((E7-F7)/E7)*100</f>
+        <v>43.599139380084715</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="104"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="40">
+        <v>61.85</v>
+      </c>
+      <c r="E8" s="40">
+        <v>29.75</v>
+      </c>
+      <c r="F8" s="40">
+        <v>3.847</v>
+      </c>
+      <c r="G8" s="40">
+        <f>+F7-F8</f>
+        <v>12.930000000000001</v>
+      </c>
+      <c r="H8" s="40">
+        <v>4.8022999999999998</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" s="52">
         <f t="shared" si="0"/>
-        <v>43.599139380084715</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="40" t="s">
+        <v>87.068907563025206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="104"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="34">
+        <v>84.18</v>
+      </c>
+      <c r="E9" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F9" s="45">
+        <v>11.09</v>
+      </c>
+      <c r="G9" s="56">
+        <f>+F7-F9</f>
+        <v>5.6870000000000012</v>
+      </c>
+      <c r="H9" s="34">
+        <v>3.8511000000000002</v>
+      </c>
+      <c r="I9" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="105">
-        <f>+F7-F8</f>
-        <v>16.777000000000001</v>
-      </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="35" t="e">
+      <c r="J9" s="35">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="105">
-        <f>+F7-F9</f>
-        <v>16.777000000000001</v>
-      </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35" t="e">
+        <v>62.722689075630257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="105"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="34">
+        <v>61.85</v>
+      </c>
+      <c r="E10" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F10" s="34">
+        <v>3.847</v>
+      </c>
+      <c r="G10" s="55">
+        <f t="shared" ref="G10" si="1">+F9-F10</f>
+        <v>7.2430000000000003</v>
+      </c>
+      <c r="H10" s="34">
+        <v>4.8022999999999998</v>
+      </c>
+      <c r="I10" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="J10" s="35">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="104">
-        <f t="shared" ref="G7:G10" si="1">+F9-F10</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>87.068907563025206</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87">
+      <c r="A11" s="101">
         <v>31</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="102" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="104"/>
+      <c r="D11" s="24">
+        <v>85.38</v>
+      </c>
+      <c r="E11" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F11" s="24">
+        <v>14.66</v>
+      </c>
+      <c r="G11" s="55"/>
       <c r="H11" s="25"/>
       <c r="I11" s="26"/>
-      <c r="J11" s="27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="J11" s="27">
+        <f>+((E11-F11)/E11)*100</f>
+        <v>50.722689075630257</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
-      <c r="B12" s="88"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="104">
+      <c r="D12" s="30">
+        <v>61.16</v>
+      </c>
+      <c r="E12" s="30">
+        <v>29.75</v>
+      </c>
+      <c r="F12" s="30">
+        <v>3.9750000000000001</v>
+      </c>
+      <c r="G12" s="55">
         <f>+F11-F12</f>
-        <v>0</v>
+        <v>10.685</v>
       </c>
       <c r="H12" s="30">
-        <v>4.0917000000000003</v>
+        <v>4.0330000000000004</v>
       </c>
       <c r="I12" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="31">
+        <f t="shared" si="0"/>
+        <v>86.638655462184872</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="J12" s="31" t="e">
+      <c r="D13" s="24">
+        <v>87.05</v>
+      </c>
+      <c r="E13" s="24">
+        <v>29.75</v>
+      </c>
+      <c r="F13" s="24">
+        <v>12.52</v>
+      </c>
+      <c r="G13" s="55">
+        <f>+F11-F13</f>
+        <v>2.1400000000000006</v>
+      </c>
+      <c r="H13" s="24">
+        <v>1.3281000000000001</v>
+      </c>
+      <c r="I13" s="24">
+        <v>0.28149999999999997</v>
+      </c>
+      <c r="J13" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="87"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="23" t="s">
+        <v>57.915966386554615</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="101"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="104">
-        <f>+F11-F13</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="24">
-        <v>0.16120000000000001</v>
-      </c>
-      <c r="I13" s="24">
-        <v>0.97489999999999999</v>
-      </c>
-      <c r="J13" s="27" t="e">
+      <c r="D14" s="34">
+        <v>61.16</v>
+      </c>
+      <c r="E14" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F14" s="34">
+        <v>3.9750000000000001</v>
+      </c>
+      <c r="G14" s="55">
+        <f>+F11-F14</f>
+        <v>10.685</v>
+      </c>
+      <c r="H14" s="34">
+        <v>4.0330000000000004</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="35">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="87"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="33" t="s">
+        <v>86.638655462184872</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="101">
+        <v>36</v>
+      </c>
+      <c r="B15" s="102" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="104">
-        <f>+F11-F14</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="34">
-        <v>4.0917000000000003</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="J14" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="87">
-        <v>36</v>
-      </c>
-      <c r="B15" s="88" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="104"/>
+      <c r="D15" s="24">
+        <v>84.13</v>
+      </c>
+      <c r="E15" s="24">
+        <v>29.75</v>
+      </c>
+      <c r="F15" s="24">
+        <v>14.21</v>
+      </c>
+      <c r="G15" s="55"/>
       <c r="H15" s="25"/>
       <c r="I15" s="26"/>
-      <c r="J15" s="27" t="e">
+      <c r="J15" s="27">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>52.235294117647058</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87"/>
-      <c r="B16" s="88"/>
+      <c r="A16" s="101"/>
+      <c r="B16" s="102"/>
       <c r="C16" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="30">
+        <v>62.65</v>
+      </c>
+      <c r="E16" s="30">
+        <v>29.75</v>
+      </c>
+      <c r="F16" s="30">
+        <v>4.1260000000000003</v>
+      </c>
+      <c r="G16" s="55">
+        <f>+F15-F16</f>
+        <v>10.084</v>
+      </c>
+      <c r="H16" s="30">
+        <v>3.6675</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16" s="31">
+        <f t="shared" si="0"/>
+        <v>86.131092436974782</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="101"/>
+      <c r="B17" s="102"/>
+      <c r="C17" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="104">
-        <f>+F15-F16</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="30">
-        <v>3.9441999999999999</v>
-      </c>
-      <c r="I16" s="30" t="s">
+      <c r="D17" s="24">
+        <v>79.77</v>
+      </c>
+      <c r="E17" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F17" s="24">
+        <v>10.43</v>
+      </c>
+      <c r="G17" s="55">
+        <f>+F15-F17</f>
+        <v>3.7800000000000011</v>
+      </c>
+      <c r="H17" s="24">
+        <v>2.8071999999999999</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="27">
+        <f t="shared" si="0"/>
+        <v>64.941176470588232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="J16" s="31" t="e">
+      <c r="D18" s="34">
+        <v>62.65</v>
+      </c>
+      <c r="E18" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F18" s="34">
+        <v>4.1260000000000003</v>
+      </c>
+      <c r="G18" s="55">
+        <f>+F15-F18</f>
+        <v>10.084</v>
+      </c>
+      <c r="H18" s="34">
+        <v>3.6675</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" s="35">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="23" t="s">
+        <v>86.131092436974782</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="101">
+        <v>38</v>
+      </c>
+      <c r="B19" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="104">
-        <f>+F15-F17</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="24">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="I17" s="24">
-        <v>0.89649999999999996</v>
-      </c>
-      <c r="J17" s="27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="33" t="s">
+      <c r="C19" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="104">
-        <f>+F15-F18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="34">
-        <v>3.9441999999999999</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" s="35" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="87">
-        <v>38</v>
-      </c>
-      <c r="B19" s="88" t="s">
-        <v>126</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="106"/>
+      <c r="D19" s="37">
+        <v>90.79</v>
+      </c>
+      <c r="E19" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F19" s="5">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="G19" s="57"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="27" t="e">
+      <c r="J19" s="27">
         <f>+((E19-F19)/E19)*100</f>
-        <v>#DIV/0!</v>
+        <v>40.67226890756303</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
-      <c r="B20" s="88"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D20" s="31">
+        <v>65.153000000000006</v>
+      </c>
+      <c r="E20" s="31">
+        <v>29.746300000000002</v>
+      </c>
+      <c r="F20" s="109">
+        <v>4.6173999999999999</v>
+      </c>
+      <c r="G20" s="57">
+        <f>+F19-F20</f>
+        <v>13.032599999999999</v>
+      </c>
+      <c r="H20" s="29">
+        <v>4.4355000000000002</v>
+      </c>
+      <c r="I20" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" s="31">
+        <f t="shared" ref="J20:J26" si="2">+((E20-F20)/E20)*100</f>
+        <v>84.477397188894074</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="5">
+        <v>94.85</v>
+      </c>
+      <c r="E21" s="34">
+        <v>29.75</v>
+      </c>
+      <c r="F21" s="5">
+        <v>15.99</v>
+      </c>
+      <c r="G21" s="57">
+        <f>+F19-F21</f>
+        <v>1.6599999999999984</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.82830000000000004</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0.5171</v>
+      </c>
+      <c r="J21" s="27">
+        <f t="shared" si="2"/>
+        <v>46.252100840336134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="101"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="106">
-        <f>+F19-F20</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="29">
-        <v>4.4191000000000003</v>
-      </c>
-      <c r="I20" s="29" t="s">
+      <c r="D22" s="33">
+        <v>65.150000000000006</v>
+      </c>
+      <c r="E22" s="33">
+        <v>29.75</v>
+      </c>
+      <c r="F22" s="33">
+        <v>4.617</v>
+      </c>
+      <c r="G22" s="57">
+        <f>+F19-F22</f>
+        <v>13.032999999999998</v>
+      </c>
+      <c r="H22" s="33">
+        <v>4.4355000000000002</v>
+      </c>
+      <c r="I22" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" s="35">
+        <f t="shared" si="2"/>
+        <v>84.480672268907568</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="101">
+        <v>43</v>
+      </c>
+      <c r="B23" s="102" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J20" s="31" t="e">
-        <f t="shared" ref="J20:J26" si="2">+((E20-F20)/E20)*100</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="106">
-        <f>+F19-F21</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0.32379999999999998</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0.89490000000000003</v>
-      </c>
-      <c r="J21" s="27" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="106">
-        <f>+F19-F22</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="33">
-        <v>4.4191000000000003</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="J22" s="35" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="87">
-        <v>43</v>
-      </c>
-      <c r="B23" s="88" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="107"/>
+      <c r="D23" s="24">
+        <v>84.5</v>
+      </c>
+      <c r="E23" s="33">
+        <v>29.75</v>
+      </c>
+      <c r="F23" s="24">
+        <v>15.08</v>
+      </c>
+      <c r="G23" s="58"/>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
-      <c r="J23" s="27" t="e">
+      <c r="J23" s="27">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>49.310924369747902</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="87"/>
-      <c r="B24" s="88"/>
+      <c r="A24" s="101"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="107">
+        <v>130</v>
+      </c>
+      <c r="D24" s="30">
+        <v>64.56</v>
+      </c>
+      <c r="E24" s="30">
+        <v>29.75</v>
+      </c>
+      <c r="F24" s="30">
+        <v>4.55</v>
+      </c>
+      <c r="G24" s="58">
         <f>+F23-F24</f>
-        <v>0</v>
+        <v>10.530000000000001</v>
       </c>
       <c r="H24" s="30">
-        <v>4.1680000000000001</v>
+        <v>3.6381999999999999</v>
       </c>
       <c r="I24" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="J24" s="31" t="e">
+        <v>145</v>
+      </c>
+      <c r="J24" s="31">
         <f>+((E24-F24)/E24)*100</f>
-        <v>#DIV/0!</v>
+        <v>84.705882352941174</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="87"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="101"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="107">
+        <v>131</v>
+      </c>
+      <c r="D25" s="24">
+        <v>88.05</v>
+      </c>
+      <c r="E25" s="33">
+        <v>29.75</v>
+      </c>
+      <c r="F25" s="24">
+        <v>13.49</v>
+      </c>
+      <c r="G25" s="58">
         <f>+F23-F25</f>
-        <v>0</v>
+        <v>1.5899999999999999</v>
       </c>
       <c r="H25" s="24">
-        <v>0.29149999999999998</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="I25" s="24">
-        <v>0.91410000000000002</v>
-      </c>
-      <c r="J25" s="27" t="e">
+        <v>0.45240000000000002</v>
+      </c>
+      <c r="J25" s="27">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>54.65546218487394</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="87"/>
-      <c r="B26" s="88"/>
+      <c r="A26" s="101"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="107">
+        <v>132</v>
+      </c>
+      <c r="D26" s="34">
+        <v>64.56</v>
+      </c>
+      <c r="E26" s="33">
+        <v>29.75</v>
+      </c>
+      <c r="F26" s="34">
+        <v>4.55</v>
+      </c>
+      <c r="G26" s="58">
         <f>+F23-F26</f>
-        <v>0</v>
+        <v>10.530000000000001</v>
       </c>
       <c r="H26" s="34">
-        <v>4.1680000000000001</v>
+        <v>3.6381999999999999</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="J26" s="35" t="e">
+        <v>145</v>
+      </c>
+      <c r="J26" s="35">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>84.705882352941174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="B23:B26"/>
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="A11:A14"/>
@@ -2906,10 +3041,13 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>